<commit_message>
Added report charts spreadsheet in Postproc folder
</commit_message>
<xml_diff>
--- a/tutorial_projects/tutorial1/cassandra/inputs/demo_project_data.xlsx
+++ b/tutorial_projects/tutorial1/cassandra/inputs/demo_project_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aa_git_repos\aa_non_code_repos\cassandra_default_road_model\tutorial_projects\tutorial1\cassandra\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52435FB3-3E6E-4BC2-BF7D-E0E5B043559C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DBD004-FFCF-4D21-A36D-C210CD202618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18780" yWindow="285" windowWidth="28530" windowHeight="19725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="budget_mono_2_5" sheetId="11" r:id="rId1"/>
@@ -1039,7 +1039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BCB7E3-4FB9-412B-BAE0-1AA1CC978545}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
@@ -3000,8 +3000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B50F2C7-8A0B-49C7-8784-FF3222E1E521}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3102,7 +3102,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Refined Post-Processing spreadsheet for training video
Refined and expanded the Excel spreadsheet in the Tutorial 1 postproc folder
</commit_message>
<xml_diff>
--- a/tutorial_projects/tutorial1/cassandra/inputs/demo_project_data.xlsx
+++ b/tutorial_projects/tutorial1/cassandra/inputs/demo_project_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aa_git_repos\aa_non_code_repos\cassandra_default_road_model\tutorial_projects\tutorial1\cassandra\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DBD004-FFCF-4D21-A36D-C210CD202618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC8474B-C432-49DB-8393-8C6654B465D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7800" yWindow="135" windowWidth="37710" windowHeight="19725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="budget_mono_2_5" sheetId="11" r:id="rId1"/>
@@ -1039,7 +1039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BCB7E3-4FB9-412B-BAE0-1AA1CC978545}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
@@ -3000,7 +3000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B50F2C7-8A0B-49C7-8784-FF3222E1E521}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -3102,7 +3102,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3322,7 +3322,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed 'median' to 'median_value' in projects setup file for kpi_set2 in tutorial1
</commit_message>
<xml_diff>
--- a/tutorial_projects/tutorial1/cassandra/inputs/demo_project_data.xlsx
+++ b/tutorial_projects/tutorial1/cassandra/inputs/demo_project_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aa_git_repos\aa_non_code_repos\cassandra_default_road_model\tutorial_projects\tutorial1\cassandra\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC8474B-C432-49DB-8393-8C6654B465D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F78A78-C5CE-4C04-BDD2-EACFF1762FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="135" windowWidth="37710" windowHeight="19725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="1155" windowWidth="37710" windowHeight="19725" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="budget_mono_2_5" sheetId="11" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="147">
   <si>
     <t>period</t>
   </si>
@@ -287,9 +287,6 @@
   </si>
   <si>
     <t>median_value</t>
-  </si>
-  <si>
-    <t>median</t>
   </si>
   <si>
     <t>1th_percentile</t>
@@ -1039,7 +1036,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BCB7E3-4FB9-412B-BAE0-1AA1CC978545}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
@@ -1055,7 +1052,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C1" s="31" t="s">
         <v>1</v>
@@ -1687,7 +1684,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C1" s="31" t="s">
         <v>1</v>
@@ -3014,77 +3011,77 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>121</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>122</v>
       </c>
       <c r="C1" s="22" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>125</v>
-      </c>
       <c r="E2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -3101,8 +3098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19816313-77C3-454A-8C23-6AF68AABAC13}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3115,196 +3112,196 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>121</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>122</v>
       </c>
       <c r="C1" s="22" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B2" s="28" t="s">
         <v>71</v>
       </c>
       <c r="C2" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" t="s">
         <v>125</v>
-      </c>
-      <c r="E2" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="B3" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>125</v>
-      </c>
       <c r="E3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="B4" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>125</v>
-      </c>
       <c r="E4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B5" s="25" t="s">
         <v>71</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B8" s="28" t="s">
         <v>71</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="B9" s="28" t="s">
-        <v>81</v>
+        <v>131</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>80</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B11" s="23" t="s">
         <v>71</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>81</v>
+        <v>132</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>80</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B14" s="28" t="s">
         <v>71</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="B15" s="28" t="s">
-        <v>81</v>
+        <v>133</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>80</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -3335,27 +3332,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="32" t="s">
         <v>136</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="D1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>140</v>
       </c>
       <c r="C2" s="33">
         <v>40</v>
@@ -3369,10 +3366,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C3" s="33">
         <v>40</v>
@@ -3386,10 +3383,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>143</v>
       </c>
       <c r="C4" s="33">
         <v>0</v>
@@ -3403,10 +3400,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>145</v>
       </c>
       <c r="C5" s="33">
         <v>10</v>
@@ -3420,10 +3417,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C6" s="33">
         <v>10</v>
@@ -3521,197 +3518,197 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added notes and hints spreadsheet
Added a Notes and Hints spreadsheet with notes about preparing the input file. Please let us keep expanding this list of 'lessons learnt' as we run into edge cases when debugging the model. The idea is for these notes to pertain to preparation of the input file to address these edge cases.
</commit_message>
<xml_diff>
--- a/tutorial_projects/tutorial1/cassandra/inputs/demo_project_data.xlsx
+++ b/tutorial_projects/tutorial1/cassandra/inputs/demo_project_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aa_git_repos\aa_non_code_repos\cassandra_default_road_model\tutorial_projects\tutorial1\cassandra\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F78A78-C5CE-4C04-BDD2-EACFF1762FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3B0821-A3BF-4F08-A429-FAB2D8F6D7B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="1155" windowWidth="37710" windowHeight="19725" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="budget_mono_2_5" sheetId="11" r:id="rId1"/>
@@ -124,9 +124,6 @@
     <t>Was 40. Minimum Surface Life Achieved to consider for AC - gatekeeper that can be used to throttle treatments</t>
   </si>
   <si>
-    <t>min_sla_to_treat_seal</t>
-  </si>
-  <si>
     <t>Minimum Surface Life Achieved to consider for Chipseals - gatekeeper that can be used to throttle treatments</t>
   </si>
   <si>
@@ -485,6 +482,9 @@
   </si>
   <si>
     <t>Renewals</t>
+  </si>
+  <si>
+    <t>min_sla_to_treat_cs</t>
   </si>
 </sst>
 </file>
@@ -1052,7 +1052,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C1" s="31" t="s">
         <v>1</v>
@@ -1684,7 +1684,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C1" s="31" t="s">
         <v>1</v>
@@ -2300,8 +2300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50F5F74A-BCC4-4AB5-9730-41F4A1723B13}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2481,13 +2481,13 @@
         <v>13</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>26</v>
+        <v>146</v>
       </c>
       <c r="C9" s="4">
         <v>50</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" s="4" t="b">
         <v>0</v>
@@ -2501,13 +2501,13 @@
         <v>13</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="4">
         <v>6</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E10" s="4" t="b">
         <v>0</v>
@@ -2521,13 +2521,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="4">
         <v>20</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" s="4" t="b">
         <v>1</v>
@@ -2541,13 +2541,13 @@
         <v>13</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" s="4">
         <v>50</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="4" t="b">
         <v>0</v>
@@ -2561,13 +2561,13 @@
         <v>13</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="4">
         <v>20</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" s="4" t="b">
         <v>0</v>
@@ -2581,13 +2581,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" s="4">
         <v>10</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" s="4" t="b">
         <v>0</v>
@@ -2618,40 +2618,40 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>58</v>
-      </c>
       <c r="C1" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="8">
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="9">
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="8">
         <v>10</v>
@@ -2660,7 +2660,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="8">
         <v>10</v>
@@ -2669,7 +2669,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="8">
         <v>10</v>
@@ -2678,7 +2678,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="9">
         <v>50</v>
@@ -2687,7 +2687,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="9">
         <v>50</v>
@@ -2696,145 +2696,145 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="8">
         <v>100</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="8">
         <v>140</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="8">
         <v>180</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="8">
         <v>120</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" s="8">
         <v>160</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" s="8">
         <v>200</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" s="9">
         <v>140</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B16" s="9">
         <v>180</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B17" s="9">
         <v>220</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B18" s="9">
         <v>160</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B19" s="9">
         <v>200</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B20" s="9">
         <v>240</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B21" s="8">
         <v>1</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2848,7 +2848,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23" s="8">
         <v>0</v>
@@ -2875,107 +2875,107 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
@@ -2985,7 +2985,7 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -3011,77 +3011,77 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>120</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>121</v>
       </c>
       <c r="C1" s="22" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>124</v>
-      </c>
       <c r="E2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -3098,7 +3098,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19816313-77C3-454A-8C23-6AF68AABAC13}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -3112,196 +3112,196 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>120</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>121</v>
       </c>
       <c r="C1" s="22" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" s="29" t="s">
+      <c r="E2" t="s">
         <v>124</v>
-      </c>
-      <c r="E2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="B3" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>124</v>
-      </c>
       <c r="E3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="B4" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>124</v>
-      </c>
       <c r="E4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="E5" t="s">
         <v>128</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="E5" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -3332,27 +3332,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="D1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>137</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>139</v>
       </c>
       <c r="C2" s="33">
         <v>40</v>
@@ -3366,10 +3366,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C3" s="33">
         <v>40</v>
@@ -3383,10 +3383,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>141</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>142</v>
       </c>
       <c r="C4" s="33">
         <v>0</v>
@@ -3400,10 +3400,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>144</v>
       </c>
       <c r="C5" s="33">
         <v>10</v>
@@ -3417,10 +3417,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C6" s="33">
         <v>10</v>
@@ -3452,263 +3452,263 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="20" t="s">
         <v>68</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>